<commit_message>
first integration of calendar with guest house, basic function working
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B18427-BA45-4AB0-A92C-99466BC7C3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,58 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>MaxBookings</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Christmas Eve</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Christmas Day</t>
+  </si>
+  <si>
+    <t>New Year's Eve</t>
+  </si>
+  <si>
+    <t>New Year's Day</t>
+  </si>
+  <si>
+    <t>Peak Season</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +105,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +392,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45650</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>18500</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45657</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>22000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45658</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45659</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>18500</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>18500</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45698</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
add initial feature to synch with excel database
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B18427-BA45-4AB0-A92C-99466BC7C3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB7BAFD-9731-4B3F-A771-ABB669196F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,16 +416,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -438,17 +438,17 @@
       <c r="C2" s="1">
         <v>18500</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -458,17 +458,17 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -481,17 +481,17 @@
       <c r="C4" s="1">
         <v>22000</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>8</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -501,17 +501,17 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -524,17 +524,17 @@
       <c r="C6" s="1">
         <v>18500</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -547,17 +547,17 @@
       <c r="C7" s="1">
         <v>18500</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
+      <c r="D7" s="1">
+        <v>10</v>
       </c>
       <c r="E7" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1">
-        <v>5</v>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -567,17 +567,17 @@
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -587,17 +587,57 @@
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45704</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45705</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename excel sheet to 1
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB7BAFD-9731-4B3F-A771-ABB669196F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9BF223-9074-4E73-BA95-923509B757C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -396,7 +396,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
rename excel sheets and update synch yml file
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9BF223-9074-4E73-BA95-923509B757C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7285D6-579A-419D-8495-7103E03325A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -396,7 +396,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
set valid input in excel for 2026
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7285D6-579A-419D-8495-7103E03325A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8C5E1-B989-4F11-83B4-446047585761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2844" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,7 +430,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>45650</v>
+        <v>46015</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45651</v>
+        <v>46016</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>45657</v>
+        <v>46022</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>45659</v>
+        <v>46024</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>45660</v>
+        <v>46025</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>45698</v>
+        <v>46063</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>45699</v>
+        <v>46064</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>45704</v>
+        <v>46069</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>45705</v>
+        <v>46070</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -638,6 +638,29 @@
       </c>
       <c r="G11" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>46082</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18500</v>
+      </c>
+      <c r="D12" s="1">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearrange the availability and booking numbers in excel for easier debugging
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA8C5E1-B989-4F11-83B4-446047585761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094D4DA8-D105-4D18-9874-C98DFFFF400D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2844" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8376" yWindow="2724" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -51,19 +51,7 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>Christmas Eve</t>
-  </si>
-  <si>
     <t>Closed</t>
-  </si>
-  <si>
-    <t>Christmas Day</t>
-  </si>
-  <si>
-    <t>New Year's Eve</t>
-  </si>
-  <si>
-    <t>New Year's Day</t>
   </si>
   <si>
     <t>Peak Season</t>
@@ -393,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,7 +418,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>46015</v>
+        <v>46076</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -439,67 +427,73 @@
         <v>18500</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>46016</v>
+        <v>46077</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>18500</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>46022</v>
+        <v>46078</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>22000</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>46023</v>
+        <v>46079</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -511,156 +505,30 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>46024</v>
+        <v>46080</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>18500</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>46025</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>18500</v>
-      </c>
-      <c r="D7" s="1">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>5</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>46063</v>
-      </c>
-      <c r="B8" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>46064</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>46069</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>46070</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>46082</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1">
-        <v>18500</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>5</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update availability: 2/16/2026, 5:18:26 PM - 8 overrides
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,9 +554,55 @@
         <v>Auto-generated from booking</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2026-02-19</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="C8">
+        <v>12800</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="C9">
+        <v>12800</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update availability: 2/16/2026, 6:19:35 PM - 6 overrides
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,80 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722CEF0E-07AC-4C31-B211-867670EA228E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>MaxBookings</t>
-  </si>
-  <si>
-    <t>Booked</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>2026-02-23</t>
-  </si>
-  <si>
-    <t>Peak Season</t>
-  </si>
-  <si>
-    <t>2026-02-24</t>
-  </si>
-  <si>
-    <t>Limited</t>
-  </si>
-  <si>
-    <t>2026-02-25</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>2026-02-26</t>
-  </si>
-  <si>
-    <t>2026-02-27</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -443,53 +396,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>MaxBookings</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Limited</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -503,16 +444,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+      <c r="G2" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2026-02-24</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Limited</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -526,16 +467,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="G3" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2026-02-25</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Closed</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -544,18 +485,18 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2026-02-26</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Closed</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -564,18 +505,18 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Closed</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -584,28 +525,38 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+        <v>2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C7">
+        <v>12800</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G1 A3:G3 A2 C2:D2 G2 A6:D6 F6:G6 A5:E5 A4:E4 G4 G5" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update availability: 7 overrides - 2/16/2026, 7:11:05 PM
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,9 +554,32 @@
         <v>Auto-generated from bookings</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C8">
+        <v>12800</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enabled calendar auto synch from excel
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,41 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5CAD61-116A-4EE8-BB25-E9EB85117D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="3828" yWindow="948" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MaxBookings</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2026-02-23</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Peak Season</t>
+  </si>
+  <si>
+    <t>2026-02-24</t>
+  </si>
+  <si>
+    <t>2026-02-25</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>2026-02-26</t>
+  </si>
+  <si>
+    <t>2026-02-27</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,41 +443,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Price</v>
-      </c>
-      <c r="D1" t="str">
-        <v>MaxBookings</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Booked</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Notes</v>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2026-02-23</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Limited</v>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -444,16 +497,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="str">
-        <v>Peak Season</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026-02-24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Limited</v>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -467,16 +520,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <v>Peak Season</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2026-02-25</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Closed</v>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -487,16 +540,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="str">
-        <v>Maintenance</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2026-02-26</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Closed</v>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -507,16 +560,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="str">
-        <v>Maintenance</v>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2026-02-27</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Closed</v>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -527,59 +580,25 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="str">
-        <v>Peak Season</v>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2026-02-22</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C7">
-        <v>12800</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2026-02-20</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C8">
-        <v>12800</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
+    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update availability: 6 overrides - 2/16/2026, 8:08:37 PM
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,80 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5CAD61-116A-4EE8-BB25-E9EB85117D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="3828" yWindow="948" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>MaxBookings</t>
-  </si>
-  <si>
-    <t>Booked</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>2026-02-23</t>
-  </si>
-  <si>
-    <t>Limited</t>
-  </si>
-  <si>
-    <t>Peak Season</t>
-  </si>
-  <si>
-    <t>2026-02-24</t>
-  </si>
-  <si>
-    <t>2026-02-25</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>2026-02-26</t>
-  </si>
-  <si>
-    <t>2026-02-27</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -443,47 +396,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>MaxBookings</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Limited</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -497,16 +444,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="G2" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2026-02-24</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Limited</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -520,16 +467,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="G3" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2026-02-25</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Closed</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -540,16 +487,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="G4" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2026-02-26</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Closed</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -560,16 +507,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="G5" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Closed</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -580,25 +527,36 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+      <c r="G6" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C7">
+        <v>12800</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
fix a bug that overwrite availability from booking
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,41 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD16B5C-5AEC-4495-A3D6-53D79691F09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="4176" yWindow="1296" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MaxBookings</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2026-02-23</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Peak Season</t>
+  </si>
+  <si>
+    <t>2026-02-24</t>
+  </si>
+  <si>
+    <t>2026-02-25</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>2026-02-26</t>
+  </si>
+  <si>
+    <t>2026-02-27</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,41 +443,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Price</v>
-      </c>
-      <c r="D1" t="str">
-        <v>MaxBookings</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Booked</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Notes</v>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2026-02-23</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Limited</v>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -444,16 +497,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="str">
-        <v>Peak Season</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026-02-24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Limited</v>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -467,16 +520,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <v>Peak Season</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2026-02-25</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Closed</v>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -487,16 +540,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="str">
-        <v>Maintenance</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2026-02-26</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Closed</v>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -507,16 +560,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="str">
-        <v>Maintenance</v>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2026-02-27</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Closed</v>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -527,36 +580,24 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="str">
-        <v>Peak Season</v>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2026-02-22</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C7">
-        <v>12800</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update Availability: 6 new records (merged with existing data)
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,80 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD16B5C-5AEC-4495-A3D6-53D79691F09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="4176" yWindow="1296" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>MaxBookings</t>
-  </si>
-  <si>
-    <t>Booked</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>2026-02-23</t>
-  </si>
-  <si>
-    <t>Limited</t>
-  </si>
-  <si>
-    <t>Peak Season</t>
-  </si>
-  <si>
-    <t>2026-02-24</t>
-  </si>
-  <si>
-    <t>2026-02-25</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>2026-02-26</t>
-  </si>
-  <si>
-    <t>2026-02-27</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -443,47 +396,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>MaxBookings</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Limited</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -497,16 +444,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="G2" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2026-02-24</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Limited</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -520,16 +467,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="G3" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2026-02-25</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Closed</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -540,16 +487,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="G4" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2026-02-26</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Closed</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -560,16 +507,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="G5" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Closed</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -580,24 +527,36 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+      <c r="G6" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C7">
+        <v>12800</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
revert content to commit a39c6c33a62e31bab7666975dcd9901af99f95ed
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,41 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C017AF41-F45C-4185-AA16-210E4FE077A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MaxBookings</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2026-02-23</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Peak Season</t>
+  </si>
+  <si>
+    <t>2026-02-24</t>
+  </si>
+  <si>
+    <t>2026-02-25</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>2026-02-26</t>
+  </si>
+  <si>
+    <t>2026-02-27</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,41 +443,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Price</v>
-      </c>
-      <c r="D1" t="str">
-        <v>MaxBookings</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Booked</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Notes</v>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2026-02-23</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Limited</v>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -444,16 +497,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="str">
-        <v>Peak Season</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026-02-24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Limited</v>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -467,16 +520,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <v>Peak Season</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2026-02-25</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Closed</v>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -487,16 +540,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="str">
-        <v>Maintenance</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2026-02-26</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Closed</v>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -507,16 +560,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="str">
-        <v>Maintenance</v>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2026-02-27</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Closed</v>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -527,36 +580,24 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="str">
-        <v>Peak Season</v>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2026-02-22</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C7">
-        <v>12800</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update availability: 6 overrides - 2/17/2026, 1:15:09 PM
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,80 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C017AF41-F45C-4185-AA16-210E4FE077A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>MaxBookings</t>
-  </si>
-  <si>
-    <t>Booked</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>2026-02-23</t>
-  </si>
-  <si>
-    <t>Limited</t>
-  </si>
-  <si>
-    <t>Peak Season</t>
-  </si>
-  <si>
-    <t>2026-02-24</t>
-  </si>
-  <si>
-    <t>2026-02-25</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>2026-02-26</t>
-  </si>
-  <si>
-    <t>2026-02-27</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -443,47 +396,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Price</v>
+      </c>
+      <c r="D1" t="str">
+        <v>MaxBookings</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Available</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Limited</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -497,16 +444,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+      <c r="G2" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2026-02-24</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Limited</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -520,16 +467,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="G3" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>2026-02-25</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Closed</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -540,16 +487,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="G4" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2026-02-26</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Closed</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -560,16 +507,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="G5" t="str">
+        <v>Maintenance</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Closed</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -580,24 +527,36 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+      <c r="G6" t="str">
+        <v>Peak Season</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C7">
+        <v>12800</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update availability: 8 overrides - 2/17/2026, 1:36:34 PM
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -554,9 +554,55 @@
         <v>Auto-generated from bookings</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2026-03-19</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Limited</v>
+      </c>
+      <c r="C8">
+        <v>12800</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Booked</v>
+      </c>
+      <c r="C9">
+        <v>12800</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Auto-generated from bookings</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
secured access token by encryption, reset excel numbers
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -1,41 +1,80 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D332CE-7A24-48DE-99A7-AADF11C3A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="31800" yWindow="3570" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MaxBookings</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>2026-02-23</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Peak Season</t>
+  </si>
+  <si>
+    <t>2026-02-24</t>
+  </si>
+  <si>
+    <t>2026-02-25</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>2026-02-26</t>
+  </si>
+  <si>
+    <t>2026-02-27</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +111,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,41 +443,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Price</v>
-      </c>
-      <c r="D1" t="str">
-        <v>MaxBookings</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Booked</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Available</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Notes</v>
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2026-02-23</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Limited</v>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -444,16 +497,16 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" t="str">
-        <v>Peak Season</v>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2026-02-24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Limited</v>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -467,16 +520,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="str">
-        <v>Peak Season</v>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2026-02-25</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Closed</v>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -487,16 +540,16 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="str">
-        <v>Maintenance</v>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2026-02-26</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Closed</v>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -507,16 +560,16 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="str">
-        <v>Maintenance</v>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2026-02-27</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Closed</v>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -527,82 +580,26 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="str">
-        <v>Peak Season</v>
+      <c r="G6" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2026-02-22</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C7">
-        <v>12800</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2026-03-19</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Limited</v>
-      </c>
-      <c r="C8">
-        <v>12800</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2026-03-20</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Booked</v>
-      </c>
-      <c r="C9">
-        <v>12800</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="str">
-        <v>Auto-generated from bookings</v>
-      </c>
-    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
+  </headerFooter>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
+    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
keep availability excel input as static, resynch calendar from excel
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D332CE-7A24-48DE-99A7-AADF11C3A185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23A634E-9651-4138-B457-B94DBB54D6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31800" yWindow="3570" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30060" yWindow="1380" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Availability" sheetId="1" r:id="rId1"/>
@@ -444,18 +444,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -501,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -524,47 +524,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>18500</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>18500</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -584,16 +590,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G3 A6:G6 A4 G4 A5 G5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
change excel dates format to m/dd/yyyy
</commit_message>
<xml_diff>
--- a/data/calendar-availability.xlsx
+++ b/data/calendar-availability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23A634E-9651-4138-B457-B94DBB54D6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DF2ED5-7D71-4991-8F00-866D53F5E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30060" yWindow="1380" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -43,31 +43,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>2026-02-23</t>
-  </si>
-  <si>
     <t>Limited</t>
   </si>
   <si>
     <t>Peak Season</t>
   </si>
   <si>
-    <t>2026-02-24</t>
-  </si>
-  <si>
-    <t>2026-02-25</t>
-  </si>
-  <si>
     <t>Closed</t>
   </si>
   <si>
     <t>Maintenance</t>
-  </si>
-  <si>
-    <t>2026-02-26</t>
-  </si>
-  <si>
-    <t>2026-02-27</t>
   </si>
 </sst>
 </file>
@@ -103,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -479,11 +465,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>46076</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2">
         <v>18500</v>
@@ -498,15 +484,15 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
+      <c r="A3" s="1">
+        <v>46077</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>18500</v>
@@ -521,15 +507,15 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
+      <c r="A4" s="1">
+        <v>46078</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>18500</v>
@@ -544,15 +530,15 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
+      <c r="A5" s="1">
+        <v>46079</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>18500</v>
@@ -567,15 +553,15 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
+      <c r="A6" s="1">
+        <v>46080</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -587,8 +573,11 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -596,7 +585,7 @@
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:G3 A6:G6 A4 G4 A5 G5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G1 B6:G6 G4 G5 B3:G3 B2:G2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>